<commit_message>
Nog wat tests in Domain
</commit_message>
<xml_diff>
--- a/TijdTmpl.xlsx
+++ b/TijdTmpl.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr date1904="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\School\2020-2021\pse\ProjectPSE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\said2\CLionProjects\ProjectPSE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87925F07-0D02-42B3-A4CB-7F3CB18A41DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8DDFF1A5-4B50-4932-B346-12C056D8DC1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,11 +34,21 @@
     <definedName name="HTML_Title" hidden="1">"Voorbeeld Tijdsblad"</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>Documentsoort:</t>
   </si>
@@ -58,25 +68,10 @@
     <t>Tijdsblad</t>
   </si>
   <si>
-    <t>PP</t>
-  </si>
-  <si>
     <t>Context:</t>
   </si>
   <si>
     <t>Project:</t>
-  </si>
-  <si>
-    <r>
-      <t>(*)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Geneva"/>
-      </rPr>
-      <t xml:space="preserve">Aan te passen </t>
-    </r>
   </si>
   <si>
     <r>
@@ -150,18 +145,6 @@
   </si>
   <si>
     <r>
-      <t>(+)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Geneva"/>
-      </rPr>
-      <t xml:space="preserve">Kolommen aan te passen </t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>Id</t>
     </r>
     <r>
@@ -209,9 +192,6 @@
     <t>Project Software Engineering</t>
   </si>
   <si>
-    <t>Sam Roggeman &amp; Said</t>
-  </si>
-  <si>
     <t xml:space="preserve">18 maart 20201 </t>
   </si>
   <si>
@@ -231,13 +211,34 @@
   </si>
   <si>
     <t>SY</t>
+  </si>
+  <si>
+    <t>Sam Roggeman &amp; Said Yandarbiev</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   3.1</t>
+  </si>
+  <si>
+    <t>Transport van Vaccins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   3.2</t>
+  </si>
+  <si>
+    <t>Vaccinatie in centrum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   3.3</t>
+  </si>
+  <si>
+    <t>Automatische simulatie</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="9"/>
       <name val="Geneva"/>
@@ -248,11 +249,6 @@
       <name val="Geneva"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="Geneva"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
       <sz val="9"/>
       <name val="Geneva"/>
     </font>
@@ -367,7 +363,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -412,9 +408,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -426,7 +419,7 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -510,7 +503,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -808,26 +801,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="11.375" defaultRowHeight="11.4"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" style="13" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="9" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="7" customWidth="1"/>
+    <col min="1" max="1" width="4.75" customWidth="1"/>
+    <col min="2" max="2" width="12.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.25" style="13" customWidth="1"/>
+    <col min="4" max="4" width="10.875" style="9" customWidth="1"/>
+    <col min="5" max="5" width="11.125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.875" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D1" s="20"/>
       <c r="E1" s="20"/>
@@ -835,10 +828,10 @@
     </row>
     <row r="2" spans="1:6">
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
@@ -860,7 +853,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D4" s="23"/>
       <c r="E4" s="23"/>
@@ -871,7 +864,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D5" s="23"/>
       <c r="E5" s="23"/>
@@ -881,8 +874,8 @@
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="27" t="s">
-        <v>21</v>
+      <c r="C6" s="26" t="s">
+        <v>25</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
@@ -892,12 +885,12 @@
       <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="30"/>
+      <c r="C7" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="29"/>
     </row>
     <row r="8" spans="1:6">
       <c r="B8" s="17"/>
@@ -906,43 +899,43 @@
       <c r="E8" s="14"/>
       <c r="F8" s="18"/>
     </row>
-    <row r="9" spans="1:6" s="6" customFormat="1" ht="13.5">
+    <row r="9" spans="1:6" s="6" customFormat="1" ht="13.8">
       <c r="A9" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
       <c r="F9" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="6" customFormat="1" ht="13.8">
+      <c r="B10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" s="6" customFormat="1" ht="13.5">
-      <c r="B10" s="5" t="s">
+      <c r="E10" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>12</v>
-      </c>
       <c r="F10" s="8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="15" customFormat="1">
       <c r="A11" s="15">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B11" s="31" t="s">
-        <v>26</v>
+      <c r="B11" s="30" t="s">
+        <v>22</v>
       </c>
       <c r="C11" s="23"/>
       <c r="D11" s="23"/>
@@ -954,7 +947,7 @@
     </row>
     <row r="12" spans="1:6">
       <c r="B12" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C12" s="13">
         <v>35469</v>
@@ -972,7 +965,7 @@
     </row>
     <row r="13" spans="1:6">
       <c r="B13" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C13" s="13">
         <v>35469</v>
@@ -990,7 +983,7 @@
     </row>
     <row r="14" spans="1:6">
       <c r="B14" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C14" s="13">
         <v>42802</v>
@@ -1007,82 +1000,72 @@
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="15">
+      <c r="B15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="13">
+        <v>42803</v>
+      </c>
+      <c r="D15" s="9">
+        <v>0.75</v>
+      </c>
+      <c r="E15" s="9">
+        <v>0.82638888888888884</v>
+      </c>
+      <c r="F15" s="7">
+        <v>7.6388888888888895E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="15">
         <v>2.1</v>
       </c>
-      <c r="B15" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="16">
-        <f>SUM(F16:F17)</f>
-        <v>0.33333333333333331</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="B16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="13">
+      <c r="B18" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="16">
+        <f>SUM(F19:IF20)</f>
+        <v>0.2222222222222221</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="B19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="13">
         <v>42802</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D19" s="9">
         <v>0.75</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E19" s="9">
         <v>0.875</v>
       </c>
-      <c r="F16" s="7">
-        <f>E16-D16</f>
+      <c r="F19" s="7">
+        <f>E19-D19</f>
         <v>0.125</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
-      <c r="B17" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="13">
-        <v>35476</v>
-      </c>
-      <c r="D17" s="9">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="E17" s="9">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="F17" s="7">
-        <f>E17-D17</f>
-        <v>0.20833333333333331</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="B18"/>
-      <c r="C18"/>
-      <c r="D18"/>
-      <c r="E18"/>
-      <c r="F18"/>
-    </row>
-    <row r="19" spans="1:6" ht="13.5">
-      <c r="A19" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-    </row>
-    <row r="20" spans="1:6" ht="13.5">
-      <c r="A20" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
+    <row r="20" spans="1:6">
+      <c r="B20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="13">
+        <v>42803</v>
+      </c>
+      <c r="D20" s="9">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E20" s="9">
+        <v>0.93055555555555547</v>
+      </c>
+      <c r="F20" s="7">
+        <f>E20-D20</f>
+        <v>9.7222222222222099E-2</v>
+      </c>
     </row>
     <row r="21" spans="1:6">
       <c r="F21"/>
@@ -1091,10 +1074,34 @@
       <c r="F22"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="F23"/>
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="7">
+        <f>SUM(F24,F25)</f>
+        <v>4.166666666666663E-2</v>
+      </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="F24"/>
+      <c r="B24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="13">
+        <v>42804</v>
+      </c>
+      <c r="D24" s="9">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E24" s="9">
+        <v>0.75</v>
+      </c>
+      <c r="F24" s="7">
+        <f>E24-D24</f>
+        <v>4.166666666666663E-2</v>
+      </c>
     </row>
     <row r="25" spans="1:6">
       <c r="F25"/>
@@ -1103,10 +1110,34 @@
       <c r="F26"/>
     </row>
     <row r="27" spans="1:6">
-      <c r="F27"/>
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" s="7">
+        <f>SUM(F28,F29)</f>
+        <v>4.1666666666666741E-2</v>
+      </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="F28"/>
+      <c r="B28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="13">
+        <v>42804</v>
+      </c>
+      <c r="D28" s="9">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E28" s="9">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F28" s="7">
+        <f>E28-D28</f>
+        <v>4.1666666666666741E-2</v>
+      </c>
     </row>
     <row r="29" spans="1:6">
       <c r="F29"/>
@@ -1115,10 +1146,34 @@
       <c r="F30"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="F31"/>
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F31" s="7">
+        <f>SUM(F32,F33)</f>
+        <v>0.125</v>
+      </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="F32"/>
+      <c r="B32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="13">
+        <v>42805</v>
+      </c>
+      <c r="D32" s="9">
+        <v>0.625</v>
+      </c>
+      <c r="E32" s="9">
+        <v>0.75</v>
+      </c>
+      <c r="F32" s="7">
+        <f>E32-D32</f>
+        <v>0.125</v>
+      </c>
     </row>
     <row r="33" spans="6:6">
       <c r="F33"/>
@@ -1133,20 +1188,18 @@
       <c r="F36"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="9">
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="C4:F4"/>
-    <mergeCell ref="A20:F20"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="C6:F6"/>
     <mergeCell ref="C7:F7"/>
-    <mergeCell ref="A19:F19"/>
     <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B18:E18"/>
   </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.74803149606299213" right="0.74803149606299213" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -1159,7 +1212,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="11.375" defaultRowHeight="11.4"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
@@ -1172,7 +1225,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="11.375" defaultRowHeight="11.4"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>